<commit_message>
Parametriza data de migração no reenquadramento
Essa data estava entremeada no código, de forma não parametrizada.
Agora, ela deve ser informada pelo usuário.
</commit_message>
<xml_diff>
--- a/reenquadramento/modelo.xlsx
+++ b/reenquadramento/modelo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cmbhfs.cmbh.mg.gov.br\rh\3. DIVPES\10. Pasta Pessoal\Gabi\orca-divpes\reenquadramento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E20F28-5B30-4DB9-9CC1-E4400D7D651F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910EA101-6CA7-4241-B57C-8748DA2BC3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="690" yWindow="1770" windowWidth="21600" windowHeight="11295" xr2:uid="{B8224C79-06D1-4697-BCAA-1536CFB6FB79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8224C79-06D1-4697-BCAA-1536CFB6FB79}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Reenquadramento dos Servidores Efetivos da CMBH</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Nota média progressão especial</t>
+  </si>
+  <si>
+    <t>Data do reenquadramento:</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +264,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -286,10 +298,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7BA7F0B-2208-48D7-A567-7EE7D5D35CEB}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,109 +638,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
+    <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="16"/>
+      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
@@ -839,84 +860,95 @@
       <c r="E28" s="5"/>
       <c r="F28" s="16"/>
     </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="16"/>
+    </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="24" t="s">
+      <c r="B30" s="4"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="14"/>
+        <v>11</v>
+      </c>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="17"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="25" t="s">
+      <c r="C36" s="17"/>
+    </row>
+    <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="12" t="s">
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="14"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C43" s="17" t="s">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="17"/>
-      <c r="E43" s="17"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="B9:F9"/>
+  <mergeCells count="10">
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="B11:F11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="C6:G6"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adiciona data que completou cond. de aposentadoria
Para CM menor que 330, completar condição de aposentadoria impede a
progressão na carreira a partir do nível 36/35. Assim, é interessante
incluir essa informação no resultado do reenquadramento.
</commit_message>
<xml_diff>
--- a/reenquadramento/modelo.xlsx
+++ b/reenquadramento/modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cmbhfs.cmbh.mg.gov.br\rh\3. DIVPES\10. Pasta Pessoal\Gabi\orca-divpes\reenquadramento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910EA101-6CA7-4241-B57C-8748DA2BC3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE384708-0557-493C-BD05-5AB261B50357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8224C79-06D1-4697-BCAA-1536CFB6FB79}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +715,7 @@
     <row r="9" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="28"/>
       <c r="C9" s="28"/>
-      <c r="D9" s="18"/>
+      <c r="D9" s="8"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
       <c r="G9" s="18"/>

</xml_diff>

<commit_message>
Remove condição de aposentadoria da progressão
Em razão de uma mudança nos pré-requisitos, a data de aposentadoria não
influencia mais a progressão na carreira. Portanto, foi removida de
todas elas.
</commit_message>
<xml_diff>
--- a/reenquadramento/modelo.xlsx
+++ b/reenquadramento/modelo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cmbhfs.cmbh.mg.gov.br\rh\3. DIVPES\10. Pasta Pessoal\Gabi\orca-divpes\reenquadramento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE384708-0557-493C-BD05-5AB261B50357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983FECD6-F522-4006-971B-1667A07AA653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B8224C79-06D1-4697-BCAA-1536CFB6FB79}"/>
   </bookViews>
@@ -39,12 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Reenquadramento dos Servidores Efetivos da CMBH</t>
-  </si>
-  <si>
-    <t>Simulação do desenvolvimento funcional e cálculo de posicionamento conforme a nova estrutura de carreira.</t>
-  </si>
-  <si>
     <t>CM:</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>Tempo sem efetivo exercício (dias):</t>
   </si>
   <si>
-    <t>Carreira simulada</t>
-  </si>
-  <si>
     <t>Data</t>
   </si>
   <si>
@@ -97,6 +88,15 @@
   </si>
   <si>
     <t>Data do reenquadramento:</t>
+  </si>
+  <si>
+    <t>Reenquadramento dos Servidores Efetivos da Câmara Municipal de Belo Horizonte</t>
+  </si>
+  <si>
+    <t>Reconstituição prospectiva da evolução funcional individual</t>
+  </si>
+  <si>
+    <t>Reenquadramento a partir da constituição prospectiva da evolução funcional individual, na forma do Título V - Disposições Transitórias, Capítulo I - Do Reenquadramento.</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,9 +637,9 @@
     <col min="7" max="7" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -650,7 +650,7 @@
     </row>
     <row r="2" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" s="25"/>
       <c r="C2" s="25"/>
@@ -661,7 +661,7 @@
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="30" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -674,7 +674,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -684,7 +684,7 @@
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -694,7 +694,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="7"/>
@@ -704,7 +704,7 @@
     </row>
     <row r="8" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="15"/>
@@ -722,7 +722,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -732,19 +732,19 @@
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -876,7 +876,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="27" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
@@ -892,25 +892,25 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C34" s="17"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C35" s="17"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C36" s="17"/>
     </row>
     <row r="37" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="29" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C37" s="29"/>
       <c r="D37" s="29"/>
@@ -918,7 +918,7 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
@@ -932,7 +932,7 @@
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C44" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D44" s="20"/>
       <c r="E44" s="20"/>

</xml_diff>